<commit_message>
added readme and cleaning contents for better presentation
</commit_message>
<xml_diff>
--- a/results_tracking.xlsx
+++ b/results_tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="-80" windowWidth="23360" windowHeight="17340" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-80" windowWidth="24080" windowHeight="17340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>same as above, but spartsity of tokens - .985 - 560 instead of 527 features from tokens</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>normal -545 features, took out I and you rates</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>only normalized pos terms, less sparce tokens, no normaized extracted features, 200 trees</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>same as above but with non normalized pos terms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Results from cross validation:</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -100,59 +112,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color indexed="40"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color indexed="62"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="63"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color indexed="11"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color indexed="62"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="62"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="9"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="11"/>
       <name val="Verdana"/>
     </font>
     <font>
@@ -166,45 +132,15 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="41"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="55"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="22"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -212,232 +148,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="9"/>
-      </left>
-      <right style="medium">
-        <color indexed="9"/>
-      </right>
-      <top style="medium">
-        <color indexed="9"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="22"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="22"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="22"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="22"/>
-      </right>
-      <top style="medium">
-        <color indexed="22"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="22"/>
-      </left>
-      <right style="medium">
-        <color indexed="22"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="22"/>
-      </right>
-      <top style="medium">
-        <color indexed="22"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="22"/>
-      </left>
-      <right style="medium">
-        <color indexed="22"/>
-      </right>
-      <top style="medium">
-        <color indexed="22"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="22"/>
-      </left>
-      <right style="medium">
-        <color indexed="22"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="22"/>
-      </left>
-      <right style="medium">
-        <color indexed="22"/>
-      </right>
-      <top style="medium">
-        <color indexed="22"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="9"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="9"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="9"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -767,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -783,7 +504,10 @@
     <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="39">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="39">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -794,17 +518,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="26">
+    <row r="4" spans="1:4" ht="26">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -815,7 +539,7 @@
         <v>0.4099043</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="26">
+    <row r="5" spans="1:4" ht="26">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -823,7 +547,7 @@
         <v>0.63297689999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="27" thickBot="1">
+    <row r="6" spans="1:4" ht="26">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -834,7 +558,7 @@
         <v>0.39347209999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="41" thickBot="1">
+    <row r="7" spans="1:4" ht="39">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -844,11 +568,11 @@
       <c r="C7">
         <v>0.39212160000000001</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>0.76036000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="52">
+    <row r="8" spans="1:4" ht="52">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -859,7 +583,7 @@
         <v>0.39324700000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="26">
+    <row r="9" spans="1:4" ht="26">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -870,7 +594,7 @@
         <v>0.39696120000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -881,7 +605,7 @@
         <v>0.392009</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="39">
+    <row r="11" spans="1:4" ht="39">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -892,7 +616,7 @@
         <v>0.39234669999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -903,7 +627,7 @@
         <v>0.39223409999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="26">
+    <row r="13" spans="1:4" ht="26">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -914,7 +638,7 @@
         <v>0.39133370000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:4">
       <c r="B14">
         <v>0.63534049999999997</v>
       </c>
@@ -922,7 +646,7 @@
         <v>0.3916714</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="18" thickBot="1">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -932,9 +656,8 @@
       <c r="C15">
         <v>0.39088349999999999</v>
       </c>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" ht="27" thickBot="1">
+    </row>
+    <row r="16" spans="1:4" ht="26">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -944,34 +667,22 @@
       <c r="C16">
         <v>0.39898709999999998</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="18"/>
-    </row>
-    <row r="17" spans="1:19" ht="16" thickBot="1">
+    </row>
+    <row r="17" spans="1:4" ht="16" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="2">
         <v>0.63792910000000003</v>
       </c>
       <c r="C17">
         <v>0.3890827</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="3">
         <v>0.75697999999999999</v>
       </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="23"/>
-    </row>
-    <row r="18" spans="1:19" ht="27" thickBot="1">
+    </row>
+    <row r="18" spans="1:4" ht="26">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -981,83 +692,38 @@
       <c r="C18">
         <v>0.38930779999999998</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:19" ht="15" thickBot="1">
-      <c r="G19" s="20"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="8"/>
-    </row>
-    <row r="20" spans="1:19" ht="15" thickBot="1">
-      <c r="G20" s="21"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="8"/>
-    </row>
-    <row r="21" spans="1:19" ht="15" thickBot="1">
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="1:19" ht="15" thickBot="1">
-      <c r="N22" s="7"/>
-      <c r="O22" s="12"/>
-    </row>
-    <row r="23" spans="1:19" ht="15" thickBot="1">
-      <c r="N23" s="7"/>
-      <c r="O23" s="12"/>
-    </row>
-    <row r="24" spans="1:19" ht="14">
-      <c r="N24" s="9"/>
-      <c r="O24" s="12"/>
-    </row>
-    <row r="25" spans="1:19" ht="14" thickBot="1"/>
-    <row r="26" spans="1:19" ht="15" thickBot="1">
-      <c r="N26" s="7"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-    </row>
-    <row r="27" spans="1:19" ht="15" thickBot="1">
-      <c r="H27" s="7"/>
-      <c r="I27" s="12"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
-    </row>
-    <row r="28" spans="1:19" ht="15" thickBot="1">
-      <c r="H28" s="7"/>
-      <c r="I28" s="12"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
-    </row>
-    <row r="29" spans="1:19" ht="14">
-      <c r="H29" s="9"/>
-      <c r="I29" s="12"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1">
+      <c r="B19">
+        <v>0.6351154</v>
+      </c>
+      <c r="C19">
+        <v>0.39043329999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="39">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0.63308949999999997</v>
+      </c>
+      <c r="C20">
+        <v>0.3927968</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="26">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0.6336522</v>
+      </c>
+      <c r="C21">
+        <v>0.39245920000000001</v>
+      </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <mergeCells count="3">
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="G17:G20"/>
-    <mergeCell ref="K17:L17"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>